<commit_message>
Added new registration test
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/testdata.xlsx
+++ b/src/main/resources/testdata/testdata.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/05622384b921d78d/Learnings/TestNGFramework/TestNGFramework/src/main/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_F25DC773A252ABDACC104887C9D872F25ADE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{708F4AE9-3C33-4E7D-8969-5719607007E5}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="11_F25DC773A252ABDACC104887C9D872F25ADE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{056073F4-60B2-444A-ACAF-671A6F1F0DDB}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Details" sheetId="1" r:id="rId1"/>
     <sheet name="Environments" sheetId="2" r:id="rId2"/>
+    <sheet name="Registration" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>Password1</t>
   </si>
@@ -46,15 +47,6 @@
     <t>Valid Password</t>
   </si>
   <si>
-    <t>ValidUser1</t>
-  </si>
-  <si>
-    <t>ValidUser2</t>
-  </si>
-  <si>
-    <t>ValidUser3</t>
-  </si>
-  <si>
     <t>Invalid Username</t>
   </si>
   <si>
@@ -89,6 +81,99 @@
   </si>
   <si>
     <t>https://uat.test.com</t>
+  </si>
+  <si>
+    <t>standard_user</t>
+  </si>
+  <si>
+    <t>locked_out_user</t>
+  </si>
+  <si>
+    <t>problem_user</t>
+  </si>
+  <si>
+    <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>R.No</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Hobbies</t>
+  </si>
+  <si>
+    <t>Languages</t>
+  </si>
+  <si>
+    <t>Skills</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>DoB Year</t>
+  </si>
+  <si>
+    <t>DoB Month</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Kiran</t>
+  </si>
+  <si>
+    <t>Kumar</t>
+  </si>
+  <si>
+    <t>Sample Address</t>
+  </si>
+  <si>
+    <t>me1@test.com</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>Scret1</t>
+  </si>
+  <si>
+    <t>Cricket;Hockey</t>
+  </si>
+  <si>
+    <t>English;Hindi</t>
+  </si>
+  <si>
+    <t>Confirm Password</t>
+  </si>
+  <si>
+    <t>DoB Day</t>
   </si>
 </sst>
 </file>
@@ -151,11 +236,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -178,6 +262,18 @@
 </file>
 
 <file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person3.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -447,7 +543,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -466,7 +562,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -474,13 +570,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
@@ -488,13 +584,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
@@ -502,13 +598,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
@@ -524,7 +620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770865FE-C21A-4D23-A020-0BAF4FC26F3C}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -536,38 +632,171 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>20</v>
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62169483-5D11-4AA4-85EC-2966D2234470}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1234567890</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" s="2">
+        <v>2000</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="2">
+        <v>20</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>